<commit_message>
multiple shell fittings for Pt
</commit_message>
<xml_diff>
--- a/structure_examples/20240806_test_original.xlsx
+++ b/structure_examples/20240806_test_original.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="O-O" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pb-Pb" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pb-O" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="O-Pb" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="O-O" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Pb-Pb" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Pb-O" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="O-Pb" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -472,8 +472,8 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>12 atoms have CN of 0
-32 atoms have CN of 1</t>
+          <t xml:space="preserve">12 atoms have CN of 0; 
+32 atoms have CN of 1; </t>
         </is>
       </c>
     </row>
@@ -491,10 +491,10 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>4 atoms have CN of 2
-18 atoms have CN of 4
-16 atoms have CN of 6
-6 atoms have CN of 8</t>
+          <t xml:space="preserve">4 atoms have CN of 2; 
+18 atoms have CN of 4; 
+16 atoms have CN of 6; 
+6 atoms have CN of 8; </t>
         </is>
       </c>
     </row>
@@ -512,8 +512,8 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>32 atoms have CN of 1
-12 atoms have CN of 2</t>
+          <t xml:space="preserve">32 atoms have CN of 1; 
+12 atoms have CN of 2; </t>
         </is>
       </c>
     </row>
@@ -531,9 +531,9 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>14 atoms have CN of 0
-20 atoms have CN of 1
-10 atoms have CN of 2</t>
+          <t xml:space="preserve">14 atoms have CN of 0; 
+20 atoms have CN of 1; 
+10 atoms have CN of 2; </t>
         </is>
       </c>
     </row>
@@ -551,9 +551,9 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>28 atoms have CN of 1
-10 atoms have CN of 2
-6 atoms have CN of 3</t>
+          <t xml:space="preserve">28 atoms have CN of 1; 
+10 atoms have CN of 2; 
+6 atoms have CN of 3; </t>
         </is>
       </c>
     </row>
@@ -571,10 +571,10 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>14 atoms have CN of 2
-8 atoms have CN of 3
-20 atoms have CN of 4
-2 atoms have CN of 6</t>
+          <t xml:space="preserve">14 atoms have CN of 2; 
+8 atoms have CN of 3; 
+20 atoms have CN of 4; 
+2 atoms have CN of 6; </t>
         </is>
       </c>
     </row>
@@ -629,12 +629,13 @@
         <v>0.1</v>
       </c>
       <c r="C2" t="n">
-        <v>1.090909090909091</v>
+        <v>0.8</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>10 atoms have CN of 1
-1 atoms have CN of 2</t>
+          <t xml:space="preserve">4 atoms have CN of 0; 
+10 atoms have CN of 1; 
+1 atoms have CN of 2; </t>
         </is>
       </c>
     </row>
@@ -648,13 +649,12 @@
         <v>0.1</v>
       </c>
       <c r="C3" t="n">
-        <v>2.909090909090909</v>
+        <v>4.266666666666667</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>8 atoms have CN of 2
-2 atoms have CN of 4
-1 atoms have CN of 8</t>
+          <t xml:space="preserve">14 atoms have CN of 4; 
+1 atoms have CN of 8; </t>
         </is>
       </c>
     </row>
@@ -668,12 +668,14 @@
         <v>0.1</v>
       </c>
       <c r="C4" t="n">
-        <v>1.454545454545455</v>
+        <v>1.6</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>3 atoms have CN of 0
-8 atoms have CN of 2</t>
+          <t xml:space="preserve">2 atoms have CN of 0; 
+4 atoms have CN of 1; 
+8 atoms have CN of 2; 
+1 atoms have CN of 4; </t>
         </is>
       </c>
     </row>
@@ -728,11 +730,12 @@
         <v>0.1</v>
       </c>
       <c r="C2" t="n">
-        <v>6</v>
+        <v>5.2</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>11 atoms have CN of 6</t>
+          <t xml:space="preserve">4 atoms have CN of 3; 
+11 atoms have CN of 6; </t>
         </is>
       </c>
     </row>
@@ -746,12 +749,12 @@
         <v>0.1</v>
       </c>
       <c r="C3" t="n">
-        <v>2.545454545454545</v>
+        <v>2.4</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>8 atoms have CN of 2
-3 atoms have CN of 4</t>
+          <t xml:space="preserve">12 atoms have CN of 2; 
+3 atoms have CN of 4; </t>
         </is>
       </c>
     </row>
@@ -765,13 +768,13 @@
         <v>0.1</v>
       </c>
       <c r="C4" t="n">
-        <v>2.545454545454545</v>
+        <v>2.4</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>6 atoms have CN of 2
-4 atoms have CN of 3
-1 atoms have CN of 4</t>
+          <t xml:space="preserve">10 atoms have CN of 2; 
+4 atoms have CN of 3; 
+1 atoms have CN of 4; </t>
         </is>
       </c>
     </row>
@@ -785,12 +788,12 @@
         <v>0.1</v>
       </c>
       <c r="C5" t="n">
-        <v>4.363636363636363</v>
+        <v>4.266666666666667</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>10 atoms have CN of 4
-1 atoms have CN of 8</t>
+          <t xml:space="preserve">14 atoms have CN of 4; 
+1 atoms have CN of 8; </t>
         </is>
       </c>
     </row>
@@ -804,13 +807,13 @@
         <v>0.1</v>
       </c>
       <c r="C6" t="n">
-        <v>0.9090909090909091</v>
+        <v>0.9333333333333333</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>4 atoms have CN of 0
-4 atoms have CN of 1
-3 atoms have CN of 2</t>
+          <t xml:space="preserve">4 atoms have CN of 0; 
+8 atoms have CN of 1; 
+3 atoms have CN of 2; </t>
         </is>
       </c>
     </row>
@@ -865,13 +868,13 @@
         <v>0.1</v>
       </c>
       <c r="C2" t="n">
-        <v>1.5</v>
+        <v>1.772727272727273</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>28 atoms have CN of 1
-10 atoms have CN of 2
-6 atoms have CN of 3</t>
+          <t xml:space="preserve">20 atoms have CN of 1; 
+14 atoms have CN of 2; 
+10 atoms have CN of 3; </t>
         </is>
       </c>
     </row>
@@ -885,13 +888,13 @@
         <v>0.1</v>
       </c>
       <c r="C3" t="n">
-        <v>0.6363636363636364</v>
+        <v>0.8181818181818182</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>20 atoms have CN of 0
-20 atoms have CN of 1
-4 atoms have CN of 2</t>
+          <t xml:space="preserve">16 atoms have CN of 0; 
+20 atoms have CN of 1; 
+8 atoms have CN of 2; </t>
         </is>
       </c>
     </row>
@@ -905,13 +908,13 @@
         <v>0.1</v>
       </c>
       <c r="C4" t="n">
-        <v>0.6363636363636364</v>
+        <v>0.8181818181818182</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>18 atoms have CN of 0
-24 atoms have CN of 1
-2 atoms have CN of 2</t>
+          <t xml:space="preserve">10 atoms have CN of 0; 
+32 atoms have CN of 1; 
+2 atoms have CN of 2; </t>
         </is>
       </c>
     </row>
@@ -925,14 +928,14 @@
         <v>0.1</v>
       </c>
       <c r="C5" t="n">
-        <v>1.090909090909091</v>
+        <v>1.454545454545455</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>18 atoms have CN of 0
-8 atoms have CN of 1
-16 atoms have CN of 2
-2 atoms have CN of 4</t>
+          <t xml:space="preserve">10 atoms have CN of 0; 
+8 atoms have CN of 1; 
+24 atoms have CN of 2; 
+2 atoms have CN of 4; </t>
         </is>
       </c>
     </row>
@@ -946,12 +949,12 @@
         <v>0.1</v>
       </c>
       <c r="C6" t="n">
-        <v>0.2272727272727273</v>
+        <v>0.3181818181818182</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>34 atoms have CN of 0
-10 atoms have CN of 1</t>
+          <t xml:space="preserve">30 atoms have CN of 0; 
+14 atoms have CN of 1; </t>
         </is>
       </c>
     </row>

</xml_diff>